<commit_message>
updated financial report 1
</commit_message>
<xml_diff>
--- a/tour/documents/finance/report-1/report-1.xlsx
+++ b/tour/documents/finance/report-1/report-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomtalbot/Desktop/Work/Third Year/Spring Term/SWENG/Finance/Financial Report 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D69240-D3D6-274F-98E5-041069E5FE31}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78C0D0A-9EBE-1141-BB8E-428AE8F23401}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15640" xr2:uid="{B8D8E330-2BFF-DD4F-A0FC-44BE34802DD9}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Individual Hours Breakdown" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Financial Report 1'!$B$1:$V$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Financial Report 1'!$B$1:$P$38</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="43">
   <si>
     <t>Spring Term</t>
   </si>
@@ -261,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -561,33 +561,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -687,9 +667,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -699,16 +676,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1045,21 +1013,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:X39"/>
+  <dimension ref="B1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="V37" sqref="B1:V37"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="12" max="12" width="25.33203125" customWidth="1"/>
-    <col min="13" max="13" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
     <col min="14" max="14" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="17" thickBot="1">
+    <row r="1" spans="2:16" ht="17" thickBot="1">
       <c r="B1" s="38" t="s">
         <v>42</v>
       </c>
@@ -1067,7 +1037,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:22">
+    <row r="2" spans="2:16">
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
       <c r="D2" s="14"/>
@@ -1076,24 +1046,18 @@
       <c r="G2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="15"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="50"/>
-    </row>
-    <row r="3" spans="2:22">
+      <c r="H2" s="15"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="15"/>
+    </row>
+    <row r="3" spans="2:16">
       <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
@@ -1112,72 +1076,48 @@
       <c r="G3" s="4">
         <v>5</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="17">
         <v>6</v>
       </c>
-      <c r="I3" s="4">
-        <v>7</v>
-      </c>
-      <c r="J3" s="4">
-        <v>8</v>
-      </c>
-      <c r="K3" s="17">
-        <v>9</v>
-      </c>
-      <c r="M3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="1">
+      <c r="K3" s="1">
         <v>1</v>
       </c>
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4</v>
+      </c>
       <c r="O3" s="2">
-        <v>2</v>
-      </c>
-      <c r="P3" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>4</v>
-      </c>
-      <c r="R3" s="2">
         <v>5</v>
       </c>
-      <c r="S3" s="2">
+      <c r="P3" s="20">
         <v>6</v>
       </c>
-      <c r="T3" s="2">
-        <v>7</v>
-      </c>
-      <c r="U3" s="2">
-        <v>8</v>
-      </c>
-      <c r="V3" s="20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22">
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="18"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="17"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="1"/>
+      <c r="H4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="20"/>
-    </row>
-    <row r="5" spans="2:22">
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" s="19" t="s">
         <v>2</v>
       </c>
@@ -1186,24 +1126,18 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="17"/>
-      <c r="M5" s="19" t="s">
+      <c r="H5" s="17"/>
+      <c r="J5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="20"/>
-    </row>
-    <row r="6" spans="2:22">
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="2:16">
       <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
@@ -1214,26 +1148,20 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="17"/>
-      <c r="M6" s="16" t="s">
+      <c r="H6" s="17"/>
+      <c r="J6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="3">
+      <c r="K6" s="3">
         <v>24000</v>
       </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="17"/>
-    </row>
-    <row r="7" spans="2:22">
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
@@ -1252,72 +1180,48 @@
       <c r="G7" s="2">
         <v>175.08</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="20">
         <v>175.08</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
         <v>175.08</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>175.08</v>
       </c>
-      <c r="K7" s="20">
+      <c r="M7" s="2">
         <v>175.08</v>
       </c>
-      <c r="M7" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="1">
+      <c r="N7" s="2">
         <v>175.08</v>
       </c>
       <c r="O7" s="2">
         <v>175.08</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="20">
         <v>175.08</v>
       </c>
-      <c r="Q7" s="2">
-        <v>175.08</v>
-      </c>
-      <c r="R7" s="2">
-        <v>175.08</v>
-      </c>
-      <c r="S7" s="2">
-        <v>175.08</v>
-      </c>
-      <c r="T7" s="2">
-        <v>175.08</v>
-      </c>
-      <c r="U7" s="2">
-        <v>175.08</v>
-      </c>
-      <c r="V7" s="20">
-        <v>175.08</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22">
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" s="18"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="21"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="8"/>
+      <c r="H8" s="21"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
       <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="24"/>
-    </row>
-    <row r="9" spans="2:22">
+      <c r="P8" s="24"/>
+    </row>
+    <row r="9" spans="2:16">
       <c r="B9" s="19" t="s">
         <v>5</v>
       </c>
@@ -1326,24 +1230,18 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="17"/>
-      <c r="M9" s="19" t="s">
+      <c r="H9" s="17"/>
+      <c r="J9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="20"/>
-    </row>
-    <row r="10" spans="2:22">
+      <c r="P9" s="20"/>
+    </row>
+    <row r="10" spans="2:16">
       <c r="B10" s="22" t="s">
         <v>6</v>
       </c>
@@ -1366,62 +1264,38 @@
         <f>10*12.5</f>
         <v>125</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="17">
         <f>10*12.5</f>
         <v>125</v>
       </c>
-      <c r="I10" s="4">
-        <f>12*12.5</f>
-        <v>150</v>
-      </c>
-      <c r="J10" s="4">
-        <f>12.5*12</f>
-        <v>150</v>
-      </c>
-      <c r="K10" s="17">
-        <f t="shared" ref="K10" si="0">16*12.5</f>
-        <v>200</v>
-      </c>
-      <c r="M10" s="22" t="s">
+      <c r="J10" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-      <c r="O10" s="7">
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
         <f>3*12.5</f>
         <v>37.5</v>
       </c>
-      <c r="P10" s="7">
+      <c r="M10" s="7">
         <f>5*12.5</f>
         <v>62.5</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="N10" s="7">
         <f>8*12.5</f>
         <v>100</v>
       </c>
-      <c r="R10" s="7">
+      <c r="O10" s="7">
         <f>8*12.5</f>
         <v>100</v>
       </c>
-      <c r="S10" s="7">
+      <c r="P10" s="21">
         <f>10*12.5</f>
         <v>125</v>
       </c>
-      <c r="T10" s="7">
-        <f>8.75*12.5</f>
-        <v>109.375</v>
-      </c>
-      <c r="U10" s="7">
-        <f>4*12.5</f>
-        <v>50</v>
-      </c>
-      <c r="V10" s="21">
-        <f>10.5*12.5</f>
-        <v>131.25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22">
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" s="18" t="s">
         <v>7</v>
       </c>
@@ -1433,229 +1307,157 @@
         <v>37.5</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" ref="E11:E14" si="1">5*12.5</f>
+        <f t="shared" ref="E11:E14" si="0">5*12.5</f>
         <v>62.5</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" ref="F11:F13" si="2">8*12.5</f>
+        <f t="shared" ref="F11:F13" si="1">8*12.5</f>
         <v>100</v>
       </c>
       <c r="G11" s="7">
         <f>7*12.5</f>
         <v>87.5</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="21">
         <f>17*12.5</f>
         <v>212.5</v>
       </c>
-      <c r="I11" s="7">
-        <f>14*12.5</f>
-        <v>175</v>
-      </c>
-      <c r="J11" s="7">
-        <f t="shared" ref="J11:K11" si="3">14*12.5</f>
-        <v>175</v>
-      </c>
-      <c r="K11" s="21">
-        <f t="shared" si="3"/>
-        <v>175</v>
-      </c>
-      <c r="M11" s="18" t="s">
+      <c r="J11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
         <f>3*12.5</f>
         <v>37.5</v>
       </c>
-      <c r="P11" s="7">
+      <c r="M11" s="7">
         <f>5*12.5</f>
         <v>62.5</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="N11" s="7">
         <f>8*12.5</f>
         <v>100</v>
       </c>
-      <c r="R11" s="7">
+      <c r="O11" s="7">
         <f>7*12.5</f>
         <v>87.5</v>
       </c>
-      <c r="S11" s="7">
+      <c r="P11" s="21">
         <f>27*12.5</f>
         <v>337.5</v>
       </c>
-      <c r="T11" s="47">
+    </row>
+    <row r="12" spans="2:16">
+      <c r="B12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" ref="D12:D16" si="2">3*12.5</f>
+        <v>37.5</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>62.5</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" ref="G12:G14" si="3">7*12.5</f>
+        <v>87.5</v>
+      </c>
+      <c r="H12" s="21">
         <f>10*12.5</f>
         <v>125</v>
       </c>
-      <c r="U11" s="47">
-        <f>13*12.5</f>
-        <v>162.5</v>
-      </c>
-      <c r="V11" s="41">
+      <c r="J12" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
+        <f>3*12.5</f>
+        <v>37.5</v>
+      </c>
+      <c r="M12" s="7">
+        <f>5*12.5</f>
+        <v>62.5</v>
+      </c>
+      <c r="N12" s="7">
+        <f>8*12.5</f>
+        <v>100</v>
+      </c>
+      <c r="O12" s="7">
+        <f>7*12.5</f>
+        <v>87.5</v>
+      </c>
+      <c r="P12" s="21">
         <f>12*12.5</f>
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="2:22">
-      <c r="B12" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7">
-        <f t="shared" ref="D12:D16" si="4">3*12.5</f>
+    <row r="13" spans="2:16">
+      <c r="B13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>62.5</v>
+      </c>
+      <c r="F13" s="7">
         <f t="shared" si="1"/>
-        <v>62.5</v>
-      </c>
-      <c r="F12" s="7">
-        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="G12" s="7">
-        <f t="shared" ref="G12:G14" si="5">7*12.5</f>
+      <c r="G13" s="7">
+        <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H12" s="7">
-        <f>10*12.5</f>
-        <v>125</v>
-      </c>
-      <c r="I12" s="7">
-        <f>12*12.5</f>
-        <v>150</v>
-      </c>
-      <c r="J12" s="7">
-        <f>12*12.5</f>
-        <v>150</v>
-      </c>
-      <c r="K12" s="21">
-        <f>14*12.5</f>
-        <v>175</v>
-      </c>
-      <c r="M12" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
-      <c r="O12" s="7">
+      <c r="H13" s="21">
+        <f t="shared" ref="H13:H14" si="4">8*12.5</f>
+        <v>100</v>
+      </c>
+      <c r="J13" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
         <f>3*12.5</f>
         <v>37.5</v>
       </c>
-      <c r="P12" s="7">
-        <f>5*12.5</f>
-        <v>62.5</v>
-      </c>
-      <c r="Q12" s="7">
-        <f>8*12.5</f>
-        <v>100</v>
-      </c>
-      <c r="R12" s="7">
+      <c r="M13" s="7">
+        <f>4*12.5</f>
+        <v>50</v>
+      </c>
+      <c r="N13" s="7">
+        <f>6.5*12.5</f>
+        <v>81.25</v>
+      </c>
+      <c r="O13" s="7">
+        <f>4.5*12.5</f>
+        <v>56.25</v>
+      </c>
+      <c r="P13" s="21">
         <f>7*12.5</f>
         <v>87.5</v>
       </c>
-      <c r="S12" s="7">
-        <f>12*12.5</f>
-        <v>150</v>
-      </c>
-      <c r="T12" s="7">
-        <f>11.5*12.5</f>
-        <v>143.75</v>
-      </c>
-      <c r="U12" s="7">
-        <f>8*12.5</f>
-        <v>100</v>
-      </c>
-      <c r="V12" s="21">
-        <f>19*12.5</f>
-        <v>237.5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22">
-      <c r="B13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
-        <f t="shared" si="4"/>
-        <v>37.5</v>
-      </c>
-      <c r="E13" s="7">
-        <f t="shared" si="1"/>
-        <v>62.5</v>
-      </c>
-      <c r="F13" s="7">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="5"/>
-        <v>87.5</v>
-      </c>
-      <c r="H13" s="7">
-        <f t="shared" ref="H13:H14" si="6">8*12.5</f>
-        <v>100</v>
-      </c>
-      <c r="I13" s="7">
-        <f>8*12.5</f>
-        <v>100</v>
-      </c>
-      <c r="J13" s="7">
-        <f>12.5*8</f>
-        <v>100</v>
-      </c>
-      <c r="K13" s="21">
-        <f t="shared" ref="K13" si="7">12*12.5</f>
-        <v>150</v>
-      </c>
-      <c r="M13" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="N13" s="6">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7">
-        <f>3*12.5</f>
-        <v>37.5</v>
-      </c>
-      <c r="P13" s="7">
-        <f>4*12.5</f>
-        <v>50</v>
-      </c>
-      <c r="Q13" s="7">
-        <f>6.5*12.5</f>
-        <v>81.25</v>
-      </c>
-      <c r="R13" s="7">
-        <f>4.5*12.5</f>
-        <v>56.25</v>
-      </c>
-      <c r="S13" s="7">
-        <f>7*12.5</f>
-        <v>87.5</v>
-      </c>
-      <c r="T13" s="7">
-        <f>9.5*12.5</f>
-        <v>118.75</v>
-      </c>
-      <c r="U13" s="7">
-        <f>11.5*12.5</f>
-        <v>143.75</v>
-      </c>
-      <c r="V13" s="21">
-        <f>15*12.5</f>
-        <v>187.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22">
+    </row>
+    <row r="14" spans="2:16">
       <c r="B14" s="18" t="s">
         <v>10</v>
       </c>
@@ -1663,11 +1465,11 @@
         <v>0</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
       <c r="F14" s="7">
@@ -1675,65 +1477,41 @@
         <v>112.5</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H14" s="7">
-        <f t="shared" si="6"/>
+      <c r="H14" s="21">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="I14" s="7">
-        <f>11*12.5</f>
-        <v>137.5</v>
-      </c>
-      <c r="J14" s="7">
-        <f>12.5*13</f>
-        <v>162.5</v>
-      </c>
-      <c r="K14" s="21">
-        <f>14*12.5</f>
-        <v>175</v>
-      </c>
-      <c r="M14" s="56" t="s">
+      <c r="J14" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="N14" s="6">
-        <v>0</v>
-      </c>
-      <c r="O14" s="7">
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
         <f>4*12.5</f>
         <v>50</v>
       </c>
-      <c r="P14" s="7">
+      <c r="M14" s="7">
         <f>5*12.5</f>
         <v>62.5</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="N14" s="7">
         <f>8*12.5</f>
         <v>100</v>
       </c>
-      <c r="R14" s="7">
+      <c r="O14" s="7">
         <f>6*12.5</f>
         <v>75</v>
       </c>
-      <c r="S14" s="7">
+      <c r="P14" s="21">
         <f>5*12.5</f>
         <v>62.5</v>
       </c>
-      <c r="T14" s="7">
-        <f>8*12.5</f>
-        <v>100</v>
-      </c>
-      <c r="U14" s="7">
-        <f>6*12.5</f>
-        <v>75</v>
-      </c>
-      <c r="V14" s="21">
-        <f>12*12.5</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22">
+    </row>
+    <row r="15" spans="2:16">
       <c r="B15" s="18" t="s">
         <v>11</v>
       </c>
@@ -1741,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="E15" s="7">
@@ -1756,62 +1534,38 @@
         <f>6*12.5</f>
         <v>75</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="21">
         <f>12*12.5</f>
         <v>150</v>
       </c>
-      <c r="I15" s="7">
-        <f t="shared" ref="I15:K15" si="8">12*12.5</f>
-        <v>150</v>
-      </c>
-      <c r="J15" s="7">
-        <f t="shared" si="8"/>
-        <v>150</v>
-      </c>
-      <c r="K15" s="21">
-        <f t="shared" si="8"/>
-        <v>150</v>
-      </c>
-      <c r="M15" s="56" t="s">
+      <c r="J15" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="N15" s="6">
-        <v>0</v>
-      </c>
-      <c r="O15" s="7">
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
         <f>3*12.5</f>
         <v>37.5</v>
       </c>
-      <c r="P15" s="7">
+      <c r="M15" s="7">
         <f>3*12.5</f>
         <v>37.5</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="N15" s="7">
         <f>8*12.5</f>
         <v>100</v>
       </c>
-      <c r="R15" s="7">
+      <c r="O15" s="7">
         <f>6*12.5</f>
         <v>75</v>
       </c>
-      <c r="S15" s="7">
+      <c r="P15" s="21">
         <f>12*12.5</f>
         <v>150</v>
       </c>
-      <c r="T15" s="7">
-        <f>10.5*12.5</f>
-        <v>131.25</v>
-      </c>
-      <c r="U15" s="7">
-        <f>7*12.5</f>
-        <v>87.5</v>
-      </c>
-      <c r="V15" s="21">
-        <f>9*12.5</f>
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22">
+    </row>
+    <row r="16" spans="2:16">
       <c r="B16" s="23" t="s">
         <v>12</v>
       </c>
@@ -1819,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="E16" s="9">
@@ -1834,62 +1588,38 @@
         <f>10*12.5</f>
         <v>125</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="24">
         <f>12*12.5</f>
         <v>150</v>
       </c>
-      <c r="I16" s="9">
-        <f>14*12.5</f>
-        <v>175</v>
-      </c>
-      <c r="J16" s="9">
-        <f>12.5*14</f>
-        <v>175</v>
-      </c>
-      <c r="K16" s="24">
-        <f t="shared" ref="K16" si="9">12.5*14</f>
-        <v>175</v>
-      </c>
-      <c r="M16" s="23" t="s">
+      <c r="J16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="6">
-        <v>0</v>
-      </c>
-      <c r="O16" s="7">
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
         <f>3*12.5</f>
         <v>37.5</v>
       </c>
-      <c r="P16" s="7">
+      <c r="M16" s="7">
         <f>5*12.5</f>
         <v>62.5</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="N16" s="7">
         <f>8*12.5</f>
         <v>100</v>
       </c>
-      <c r="R16" s="7">
+      <c r="O16" s="7">
         <f>12*12.5</f>
         <v>150</v>
       </c>
-      <c r="S16" s="7">
+      <c r="P16" s="21">
         <f>12*12.5</f>
         <v>150</v>
       </c>
-      <c r="T16" s="7">
-        <f>14*12.5</f>
-        <v>175</v>
-      </c>
-      <c r="U16" s="7">
-        <f t="shared" ref="U16:V16" si="10">14*12.5</f>
-        <v>175</v>
-      </c>
-      <c r="V16" s="21">
-        <f t="shared" si="10"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="2:24">
+    </row>
+    <row r="17" spans="2:18">
       <c r="B17" s="25" t="s">
         <v>13</v>
       </c>
@@ -1905,69 +1635,45 @@
         <v>412.5</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" ref="F17:K17" si="11">SUM(F10:F16)</f>
+        <f t="shared" ref="F17:H17" si="5">SUM(F10:F16)</f>
         <v>712.5</v>
       </c>
       <c r="G17" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>675</v>
       </c>
-      <c r="H17" s="7">
-        <f t="shared" si="11"/>
+      <c r="H17" s="21">
+        <f t="shared" si="5"/>
         <v>962.5</v>
       </c>
-      <c r="I17" s="7">
-        <f t="shared" si="11"/>
-        <v>1037.5</v>
-      </c>
-      <c r="J17" s="7">
-        <f t="shared" si="11"/>
+      <c r="J17" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" ref="L17:P17" si="6">SUM(L10:L16)</f>
+        <v>275</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="6"/>
+        <v>681.25</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="6"/>
+        <v>631.25</v>
+      </c>
+      <c r="P17" s="20">
+        <f t="shared" si="6"/>
         <v>1062.5</v>
       </c>
-      <c r="K17" s="21">
-        <f t="shared" si="11"/>
-        <v>1200</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O17" s="2">
-        <f t="shared" ref="O17:T17" si="12">SUM(O10:O16)</f>
-        <v>275</v>
-      </c>
-      <c r="P17" s="2">
-        <f t="shared" si="12"/>
-        <v>400</v>
-      </c>
-      <c r="Q17" s="2">
-        <f t="shared" si="12"/>
-        <v>681.25</v>
-      </c>
-      <c r="R17" s="2">
-        <f t="shared" si="12"/>
-        <v>631.25</v>
-      </c>
-      <c r="S17" s="2">
-        <f t="shared" si="12"/>
-        <v>1062.5</v>
-      </c>
-      <c r="T17" s="2">
-        <f t="shared" si="12"/>
-        <v>903.125</v>
-      </c>
-      <c r="U17" s="2">
-        <f t="shared" ref="U17:V17" si="13">SUM(U10:U16)</f>
-        <v>793.75</v>
-      </c>
-      <c r="V17" s="20">
-        <f t="shared" si="13"/>
-        <v>1143.75</v>
-      </c>
-    </row>
-    <row r="18" spans="2:24">
+    </row>
+    <row r="18" spans="2:18">
       <c r="B18" s="26" t="s">
         <v>15</v>
       </c>
@@ -1978,94 +1684,64 @@
         <v>14</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" ref="E18:K18" si="14">D17</f>
+        <f t="shared" ref="E18:H18" si="7">D17</f>
         <v>262.5</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>412.5</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>712.5</v>
       </c>
-      <c r="H18" s="2">
-        <f t="shared" si="14"/>
+      <c r="H18" s="20">
+        <f t="shared" si="7"/>
         <v>675</v>
       </c>
-      <c r="I18" s="2">
-        <f t="shared" si="14"/>
-        <v>962.5</v>
-      </c>
-      <c r="J18" s="2">
-        <f t="shared" si="14"/>
-        <v>1037.5</v>
-      </c>
-      <c r="K18" s="20">
-        <f t="shared" si="14"/>
-        <v>1062.5</v>
-      </c>
-      <c r="M18" s="26" t="s">
+      <c r="J18" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P18" s="7">
+      <c r="K18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="7">
+        <f>L17</f>
+        <v>275</v>
+      </c>
+      <c r="N18" s="7">
+        <f>M17</f>
+        <v>400</v>
+      </c>
+      <c r="O18" s="7">
+        <f>N17</f>
+        <v>681.25</v>
+      </c>
+      <c r="P18" s="21">
         <f>O17</f>
-        <v>275</v>
-      </c>
-      <c r="Q18" s="7">
-        <f>P17</f>
-        <v>400</v>
-      </c>
-      <c r="R18" s="7">
-        <f>Q17</f>
-        <v>681.25</v>
-      </c>
-      <c r="S18" s="7">
-        <f>R17</f>
         <v>631.25</v>
       </c>
-      <c r="T18" s="7">
-        <f>S17</f>
-        <v>1062.5</v>
-      </c>
-      <c r="U18" s="7">
-        <f t="shared" ref="U18:V18" si="15">T17</f>
-        <v>903.125</v>
-      </c>
-      <c r="V18" s="21">
-        <f t="shared" si="15"/>
-        <v>793.75</v>
-      </c>
-    </row>
-    <row r="19" spans="2:24">
+    </row>
+    <row r="19" spans="2:18">
       <c r="B19" s="26"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="27"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="10"/>
+      <c r="H19" s="27"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
       <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="27"/>
-    </row>
-    <row r="20" spans="2:24">
+      <c r="P19" s="27"/>
+    </row>
+    <row r="20" spans="2:18">
       <c r="B20" s="26" t="s">
         <v>16</v>
       </c>
@@ -2084,50 +1760,32 @@
       <c r="G20" s="2">
         <v>632.69000000000005</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="20">
         <v>632.69000000000005</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="6">
         <v>632.69000000000005</v>
       </c>
-      <c r="J20" s="2">
+      <c r="L20" s="7">
         <v>632.69000000000005</v>
       </c>
-      <c r="K20" s="20">
+      <c r="M20" s="7">
         <v>632.69000000000005</v>
       </c>
-      <c r="M20" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20" s="6">
+      <c r="N20" s="7">
         <v>632.69000000000005</v>
       </c>
       <c r="O20" s="7">
         <v>632.69000000000005</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="21">
         <v>632.69000000000005</v>
       </c>
-      <c r="Q20" s="7">
-        <v>632.69000000000005</v>
-      </c>
-      <c r="R20" s="7">
-        <v>632.69000000000005</v>
-      </c>
-      <c r="S20" s="7">
-        <v>632.69000000000005</v>
-      </c>
-      <c r="T20" s="7">
-        <v>632.69000000000005</v>
-      </c>
-      <c r="U20" s="7">
-        <v>633.69000000000005</v>
-      </c>
-      <c r="V20" s="21">
-        <v>634.69000000000005</v>
-      </c>
-    </row>
-    <row r="21" spans="2:24">
+    </row>
+    <row r="21" spans="2:18">
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
@@ -2147,79 +1805,53 @@
       <c r="G21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="2">
-        <f>SUM(G20:I20)</f>
-        <v>1898.0700000000002</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" s="26" t="s">
+      <c r="H21" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>14</v>
+      <c r="K21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="2">
+        <f>SUM(K20:N20)</f>
+        <v>2530.7600000000002</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q21" s="2">
-        <f>SUM(N20:Q20)</f>
-        <v>2530.7600000000002</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T21" s="2">
-        <f>SUM(R20:T20)</f>
-        <v>1898.0700000000002</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V21" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-    </row>
-    <row r="22" spans="2:24">
+      <c r="P21" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+    </row>
+    <row r="22" spans="2:18">
       <c r="B22" s="25"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="27"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="45"/>
-      <c r="U22" s="45"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="55"/>
-      <c r="X22" s="55"/>
-    </row>
-    <row r="23" spans="2:24">
+      <c r="H22" s="27"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
+    </row>
+    <row r="23" spans="2:18">
       <c r="B23" s="26" t="s">
         <v>18</v>
       </c>
@@ -2238,52 +1870,34 @@
       <c r="G23" s="2">
         <v>100</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="20">
         <v>100</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="1">
         <v>100</v>
       </c>
-      <c r="J23" s="2">
+      <c r="L23" s="2">
         <v>100</v>
       </c>
-      <c r="K23" s="20">
+      <c r="M23" s="2">
         <v>100</v>
       </c>
-      <c r="M23" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="N23" s="1">
+      <c r="N23" s="2">
         <v>100</v>
       </c>
       <c r="O23" s="2">
         <v>100</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P23" s="20">
         <v>100</v>
       </c>
-      <c r="Q23" s="2">
-        <v>100</v>
-      </c>
-      <c r="R23" s="2">
-        <v>100</v>
-      </c>
-      <c r="S23" s="2">
-        <v>100</v>
-      </c>
-      <c r="T23" s="2">
-        <v>100</v>
-      </c>
-      <c r="U23" s="2">
-        <v>101</v>
-      </c>
-      <c r="V23" s="20">
-        <v>102</v>
-      </c>
-      <c r="W23" s="55"/>
-      <c r="X23" s="55"/>
-    </row>
-    <row r="24" spans="2:24">
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+    </row>
+    <row r="24" spans="2:18">
       <c r="B24" s="26" t="s">
         <v>19</v>
       </c>
@@ -2302,72 +1916,48 @@
       <c r="G24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="20">
         <v>600</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M24" s="26" t="s">
+      <c r="J24" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="K24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" s="7" t="s">
         <v>14</v>
       </c>
       <c r="O24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S24" s="7">
+      <c r="P24" s="21">
         <v>600</v>
       </c>
-      <c r="T24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="U24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="V24" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:24">
+    </row>
+    <row r="25" spans="2:18">
       <c r="B25" s="18"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="21"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="1"/>
+      <c r="H25" s="21"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="20"/>
-    </row>
-    <row r="26" spans="2:24">
+      <c r="P25" s="20"/>
+    </row>
+    <row r="26" spans="2:18">
       <c r="B26" s="26" t="s">
         <v>20</v>
       </c>
@@ -2386,50 +1976,32 @@
       <c r="G26" s="4">
         <v>50</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="17">
         <v>50</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="6">
         <v>50</v>
       </c>
-      <c r="J26" s="4">
+      <c r="L26" s="7">
         <v>50</v>
       </c>
-      <c r="K26" s="17">
+      <c r="M26" s="7">
         <v>50</v>
       </c>
-      <c r="M26" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="N26" s="6">
+      <c r="N26" s="7">
         <v>50</v>
       </c>
       <c r="O26" s="7">
         <v>50</v>
       </c>
-      <c r="P26" s="7">
+      <c r="P26" s="21">
         <v>50</v>
       </c>
-      <c r="Q26" s="7">
-        <v>50</v>
-      </c>
-      <c r="R26" s="7">
-        <v>50</v>
-      </c>
-      <c r="S26" s="7">
-        <v>50</v>
-      </c>
-      <c r="T26" s="7">
-        <v>50</v>
-      </c>
-      <c r="U26" s="7">
-        <v>51</v>
-      </c>
-      <c r="V26" s="21">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="2:24">
+    </row>
+    <row r="27" spans="2:18">
       <c r="B27" s="26" t="s">
         <v>21</v>
       </c>
@@ -2448,72 +2020,48 @@
       <c r="G27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="20">
         <v>300</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M27" s="26" t="s">
+      <c r="J27" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="K27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S27" s="2">
+      <c r="P27" s="20">
         <v>300</v>
       </c>
-      <c r="T27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V27" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="2:24">
+    </row>
+    <row r="28" spans="2:18">
       <c r="B28" s="18"/>
       <c r="C28" s="5"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="21"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="5"/>
+      <c r="H28" s="21"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
       <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="21"/>
-    </row>
-    <row r="29" spans="2:24">
+      <c r="P28" s="21"/>
+    </row>
+    <row r="29" spans="2:18">
       <c r="B29" s="26" t="s">
         <v>40</v>
       </c>
@@ -2532,50 +2080,32 @@
       <c r="G29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="2">
-        <v>500</v>
-      </c>
-      <c r="K29" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M29" s="26" t="s">
+      <c r="H29" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="K29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="O29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U29" s="2">
-        <v>750</v>
-      </c>
-      <c r="V29" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="2:24">
+      <c r="P29" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18">
       <c r="B30" s="26" t="s">
         <v>41</v>
       </c>
@@ -2594,73 +2124,48 @@
       <c r="G30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="2">
-        <v>500</v>
-      </c>
-      <c r="K30" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M30" s="44" t="s">
+      <c r="H30" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="O30" s="48" t="s">
+      <c r="K30" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="O30" s="46" t="s">
         <v>14</v>
       </c>
       <c r="P30" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="Q30" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="R30" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="S30" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="T30" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="U30" s="48">
-        <f>750+125+375</f>
-        <v>1250</v>
-      </c>
-      <c r="V30" s="52" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="2:24">
+    </row>
+    <row r="31" spans="2:18">
       <c r="B31" s="18"/>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="21"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="1"/>
+      <c r="H31" s="21"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="20"/>
-    </row>
-    <row r="32" spans="2:24">
+      <c r="P31" s="20"/>
+    </row>
+    <row r="32" spans="2:18">
       <c r="B32" s="26" t="s">
         <v>22</v>
       </c>
@@ -2679,46 +2184,28 @@
       <c r="G32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="26" t="s">
+      <c r="H32" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="N32" s="6" t="s">
+      <c r="K32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N32" s="7" t="s">
         <v>14</v>
       </c>
       <c r="O32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="R32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="T32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="U32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="V32" s="21" t="s">
+      <c r="P32" s="21" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2729,20 +2216,14 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="24"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="1"/>
+      <c r="H33" s="24"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="20"/>
+      <c r="P33" s="20"/>
     </row>
     <row r="34" spans="2:23">
       <c r="B34" s="26" t="s">
@@ -2768,60 +2249,36 @@
         <f>SUM(F17+G7)</f>
         <v>887.58</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="20">
         <f>SUM(C26:H26)+SUM(C23:H23)+G17+H7</f>
         <v>1750.08</v>
       </c>
-      <c r="I34" s="2">
-        <f>H17+SUM(G20:I20)+I7</f>
-        <v>3035.65</v>
-      </c>
-      <c r="J34" s="2">
-        <f>I17+J29+J7</f>
-        <v>1712.58</v>
-      </c>
-      <c r="K34" s="20">
-        <f>J17+K7</f>
-        <v>1237.58</v>
-      </c>
-      <c r="M34" s="26" t="s">
+      <c r="J34" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="N34" s="6">
-        <f>SUM(N7)</f>
+      <c r="K34" s="6">
+        <f>SUM(K7)</f>
         <v>175.08</v>
+      </c>
+      <c r="L34" s="7">
+        <f>SUM(L7+L17)</f>
+        <v>450.08000000000004</v>
+      </c>
+      <c r="M34" s="7">
+        <f>SUM(M7+M17)</f>
+        <v>575.08000000000004</v>
+      </c>
+      <c r="N34" s="7">
+        <f>SUM(N7+N17+N21)</f>
+        <v>3387.09</v>
       </c>
       <c r="O34" s="7">
         <f>SUM(O7+O17)</f>
-        <v>450.08000000000004</v>
-      </c>
-      <c r="P34" s="7">
-        <f>SUM(P7+P17)</f>
-        <v>575.08000000000004</v>
-      </c>
-      <c r="Q34" s="7">
-        <f>SUM(Q7+Q17+Q21)</f>
-        <v>3387.09</v>
-      </c>
-      <c r="R34" s="7">
-        <f>SUM(R7+R17)</f>
         <v>806.33</v>
       </c>
-      <c r="S34" s="7">
-        <f>SUM(S7+S17)+S24+S27</f>
+      <c r="P34" s="21">
+        <f>SUM(P7+P17)+P24+P27</f>
         <v>2137.58</v>
-      </c>
-      <c r="T34" s="7">
-        <f>SUM(T7+T17+T21)</f>
-        <v>2976.2750000000001</v>
-      </c>
-      <c r="U34" s="7">
-        <f>SUM(U7+U17-U30+U29)</f>
-        <v>468.83000000000004</v>
-      </c>
-      <c r="V34" s="21">
-        <f t="shared" ref="V34" si="16">SUM(V7+V17)</f>
-        <v>1318.83</v>
       </c>
     </row>
     <row r="35" spans="2:23">
@@ -2831,20 +2288,14 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="21"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="1"/>
+      <c r="H35" s="21"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="20"/>
+      <c r="P35" s="20"/>
     </row>
     <row r="36" spans="2:23">
       <c r="B36" s="28" t="s">
@@ -2863,67 +2314,43 @@
         <v>23649.839999999997</v>
       </c>
       <c r="F36" s="4">
-        <f t="shared" ref="F36:K36" si="17">E37</f>
+        <f t="shared" ref="F36:H36" si="8">E37</f>
         <v>23212.259999999995</v>
       </c>
       <c r="G36" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>20093.919999999995</v>
       </c>
-      <c r="H36" s="4">
-        <f t="shared" si="17"/>
+      <c r="H36" s="17">
+        <f t="shared" si="8"/>
         <v>19206.339999999993</v>
       </c>
-      <c r="I36" s="4">
-        <f t="shared" si="17"/>
-        <v>17456.259999999995</v>
-      </c>
-      <c r="J36" s="4">
-        <f t="shared" si="17"/>
-        <v>14420.609999999995</v>
-      </c>
-      <c r="K36" s="17">
-        <f t="shared" si="17"/>
-        <v>12708.029999999995</v>
-      </c>
-      <c r="M36" s="28" t="s">
+      <c r="J36" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="N36" s="6">
-        <f>N6</f>
+      <c r="K36" s="6">
+        <f>K6</f>
         <v>24000</v>
       </c>
+      <c r="L36" s="7">
+        <f t="shared" ref="L36:P36" si="9">K37</f>
+        <v>23824.92</v>
+      </c>
+      <c r="M36" s="7">
+        <f t="shared" si="9"/>
+        <v>23374.839999999997</v>
+      </c>
+      <c r="N36" s="7">
+        <f t="shared" si="9"/>
+        <v>22799.759999999995</v>
+      </c>
       <c r="O36" s="7">
-        <f t="shared" ref="O36:T36" si="18">N37</f>
-        <v>23824.92</v>
-      </c>
-      <c r="P36" s="7">
-        <f t="shared" si="18"/>
-        <v>23374.839999999997</v>
-      </c>
-      <c r="Q36" s="7">
-        <f t="shared" si="18"/>
-        <v>22799.759999999995</v>
-      </c>
-      <c r="R36" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>19412.669999999995</v>
       </c>
-      <c r="S36" s="7">
-        <f t="shared" si="18"/>
+      <c r="P36" s="21">
+        <f t="shared" si="9"/>
         <v>18606.339999999993</v>
-      </c>
-      <c r="T36" s="7">
-        <f t="shared" si="18"/>
-        <v>16468.759999999995</v>
-      </c>
-      <c r="U36" s="7">
-        <f t="shared" ref="U36" si="19">T37</f>
-        <v>13492.484999999995</v>
-      </c>
-      <c r="V36" s="21">
-        <f t="shared" ref="V36" si="20">U37</f>
-        <v>13023.654999999995</v>
       </c>
     </row>
     <row r="37" spans="2:23" ht="17" thickBot="1">
@@ -2939,75 +2366,51 @@
         <v>23649.839999999997</v>
       </c>
       <c r="E37" s="31">
-        <f t="shared" ref="E37:K37" si="21">E36-E34</f>
+        <f t="shared" ref="E37:H37" si="10">E36-E34</f>
         <v>23212.259999999995</v>
       </c>
       <c r="F37" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="10"/>
         <v>20093.919999999995</v>
       </c>
       <c r="G37" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="10"/>
         <v>19206.339999999993</v>
       </c>
-      <c r="H37" s="31">
-        <f t="shared" si="21"/>
+      <c r="H37" s="32">
+        <f t="shared" si="10"/>
         <v>17456.259999999995</v>
       </c>
-      <c r="I37" s="31">
-        <f t="shared" si="21"/>
-        <v>14420.609999999995</v>
-      </c>
-      <c r="J37" s="31">
-        <f t="shared" si="21"/>
-        <v>12708.029999999995</v>
-      </c>
-      <c r="K37" s="32">
-        <f t="shared" si="21"/>
-        <v>11470.449999999995</v>
-      </c>
-      <c r="M37" s="29" t="s">
+      <c r="J37" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="N37" s="30">
-        <f t="shared" ref="N37:T37" si="22">N36-N34</f>
+      <c r="K37" s="30">
+        <f t="shared" ref="K37:P37" si="11">K36-K34</f>
         <v>23824.92</v>
       </c>
+      <c r="L37" s="31">
+        <f t="shared" si="11"/>
+        <v>23374.839999999997</v>
+      </c>
+      <c r="M37" s="31">
+        <f t="shared" si="11"/>
+        <v>22799.759999999995</v>
+      </c>
+      <c r="N37" s="31">
+        <f t="shared" si="11"/>
+        <v>19412.669999999995</v>
+      </c>
       <c r="O37" s="31">
-        <f t="shared" si="22"/>
-        <v>23374.839999999997</v>
-      </c>
-      <c r="P37" s="31">
-        <f t="shared" si="22"/>
-        <v>22799.759999999995</v>
-      </c>
-      <c r="Q37" s="31">
-        <f t="shared" si="22"/>
-        <v>19412.669999999995</v>
-      </c>
-      <c r="R37" s="31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="11"/>
         <v>18606.339999999993</v>
       </c>
-      <c r="S37" s="31">
-        <f t="shared" si="22"/>
+      <c r="P37" s="32">
+        <f t="shared" si="11"/>
         <v>16468.759999999995</v>
       </c>
-      <c r="T37" s="31">
-        <f t="shared" si="22"/>
-        <v>13492.484999999995</v>
-      </c>
-      <c r="U37" s="31">
-        <f t="shared" ref="U37:V37" si="23">U36-U34</f>
-        <v>13023.654999999995</v>
-      </c>
-      <c r="V37" s="32">
-        <f t="shared" si="23"/>
-        <v>11704.824999999995</v>
-      </c>
     </row>
     <row r="38" spans="2:23">
-      <c r="B38" s="46"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -3017,35 +2420,35 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="55"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="55"/>
-      <c r="P38" s="55"/>
-      <c r="Q38" s="55"/>
-      <c r="R38" s="55"/>
-      <c r="S38" s="55"/>
-      <c r="T38" s="55"/>
-      <c r="U38" s="55"/>
-      <c r="V38" s="55"/>
-      <c r="W38" s="55"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="51"/>
+      <c r="T38" s="51"/>
+      <c r="U38" s="51"/>
+      <c r="V38" s="51"/>
+      <c r="W38" s="51"/>
     </row>
     <row r="39" spans="2:23">
-      <c r="M39" s="55"/>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="55"/>
-      <c r="Q39" s="55"/>
-      <c r="R39" s="55"/>
-      <c r="S39" s="55"/>
-      <c r="T39" s="55"/>
-      <c r="U39" s="55"/>
-      <c r="V39" s="55"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="51"/>
+      <c r="V39" s="51"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6l9Jk7v38KySS2vp3xsY98yHESlUD2MyTuk629JlikCoXv/qPGaplI21KGo31Me1YQANduPZBG7Io+JQ2jViLg==" saltValue="NKeU6uNmORtQaiy6hz63Lw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oQ0DwcwXpNKen4P7OC71rMeizPq5fTxPTqXFyBAh9BHvGb3BXQQnDpwMeg2bZiStyYeZPbmg8jLtI3KanFqfhg==" saltValue="xqFkvZ2EkxNnMOjXKj0VIw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="44" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3064,14 +2467,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:23" ht="20">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="N4" s="57" t="s">
+      <c r="C4" s="53"/>
+      <c r="N4" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="57"/>
+      <c r="O4" s="53"/>
     </row>
     <row r="5" spans="1:23" ht="18" thickBot="1">
       <c r="B5" s="33" t="s">
@@ -3189,7 +2592,7 @@
       <c r="R6" s="35">
         <v>0</v>
       </c>
-      <c r="S6" s="43">
+      <c r="S6" s="42">
         <v>0</v>
       </c>
       <c r="T6" s="35">
@@ -3261,7 +2664,7 @@
       <c r="R7" s="35">
         <v>3</v>
       </c>
-      <c r="S7" s="43">
+      <c r="S7" s="42">
         <v>3</v>
       </c>
       <c r="T7" s="35">
@@ -3333,7 +2736,7 @@
       <c r="R8">
         <v>5</v>
       </c>
-      <c r="S8" s="42">
+      <c r="S8" s="41">
         <v>3</v>
       </c>
       <c r="T8">
@@ -3405,7 +2808,7 @@
       <c r="R9">
         <v>8</v>
       </c>
-      <c r="S9" s="42">
+      <c r="S9" s="41">
         <v>8</v>
       </c>
       <c r="T9">
@@ -3477,7 +2880,7 @@
       <c r="R10">
         <v>7</v>
       </c>
-      <c r="S10" s="42">
+      <c r="S10" s="41">
         <v>6</v>
       </c>
       <c r="T10">
@@ -3537,7 +2940,7 @@
       <c r="N11" s="34">
         <v>43143</v>
       </c>
-      <c r="O11" s="42">
+      <c r="O11" s="41">
         <v>10</v>
       </c>
       <c r="P11">
@@ -3549,7 +2952,7 @@
       <c r="R11">
         <v>27</v>
       </c>
-      <c r="S11" s="42">
+      <c r="S11" s="41">
         <v>12</v>
       </c>
       <c r="T11" s="40">
@@ -3609,7 +3012,7 @@
       <c r="N12" s="34">
         <v>43150</v>
       </c>
-      <c r="O12" s="42">
+      <c r="O12" s="41">
         <v>8.75</v>
       </c>
       <c r="P12">
@@ -3618,10 +3021,10 @@
       <c r="Q12">
         <v>9.5</v>
       </c>
-      <c r="R12" s="42">
+      <c r="R12" s="41">
         <v>10</v>
       </c>
-      <c r="S12" s="42">
+      <c r="S12" s="41">
         <v>10.5</v>
       </c>
       <c r="T12">
@@ -3681,7 +3084,7 @@
       <c r="N13" s="34">
         <v>43157</v>
       </c>
-      <c r="O13" s="42">
+      <c r="O13" s="41">
         <v>4</v>
       </c>
       <c r="P13">
@@ -3690,10 +3093,10 @@
       <c r="Q13">
         <v>11.5</v>
       </c>
-      <c r="R13" s="42">
+      <c r="R13" s="41">
         <v>13</v>
       </c>
-      <c r="S13" s="42">
+      <c r="S13" s="41">
         <v>7</v>
       </c>
       <c r="T13">
@@ -3753,7 +3156,7 @@
       <c r="N14" s="34">
         <v>43164</v>
       </c>
-      <c r="O14" s="42">
+      <c r="O14" s="41">
         <v>10.5</v>
       </c>
       <c r="P14">
@@ -3762,10 +3165,10 @@
       <c r="Q14">
         <v>15</v>
       </c>
-      <c r="R14" s="42">
+      <c r="R14" s="41">
         <v>12</v>
       </c>
-      <c r="S14" s="42">
+      <c r="S14" s="41">
         <v>9</v>
       </c>
       <c r="T14">

</xml_diff>